<commit_message>
gamble first run second try
</commit_message>
<xml_diff>
--- a/src/workflow-colab/Editados/Apuestas/Config Workflow.xlsx
+++ b/src/workflow-colab/Editados/Apuestas/Config Workflow.xlsx
@@ -8,12 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\guido\Desktop\CD03\dm2023a\src\workflow-colab\Editados\Apuestas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8ED48CCD-8886-4D1C-A80B-03782B3430D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98B53FE8-65E4-4228-AFEE-C4D9D786F496}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="3165" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15620" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="FE" sheetId="2" r:id="rId2"/>
+    <sheet name="TS" sheetId="3" r:id="rId3"/>
+    <sheet name="HT" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="72">
   <si>
     <t>Archivo</t>
   </si>
@@ -75,6 +78,183 @@
   </si>
   <si>
     <t>20211 en adelante</t>
+  </si>
+  <si>
+    <t>FE01</t>
+  </si>
+  <si>
+    <t>Feature Engineering</t>
+  </si>
+  <si>
+    <t>Versión</t>
+  </si>
+  <si>
+    <t>num.trees</t>
+  </si>
+  <si>
+    <t>max.depth</t>
+  </si>
+  <si>
+    <t>min.node.size</t>
+  </si>
+  <si>
+    <t>mtry</t>
+  </si>
+  <si>
+    <t>semilla</t>
+  </si>
+  <si>
+    <t>Canarios</t>
+  </si>
+  <si>
+    <t>lag1</t>
+  </si>
+  <si>
+    <t>lag2</t>
+  </si>
+  <si>
+    <t>lag3</t>
+  </si>
+  <si>
+    <t>Tendencias1</t>
+  </si>
+  <si>
+    <t>Tendencias2</t>
+  </si>
+  <si>
+    <t>Todo TRUE</t>
+  </si>
+  <si>
+    <t>Training Strategy</t>
+  </si>
+  <si>
+    <t>future</t>
+  </si>
+  <si>
+    <t>final_train</t>
+  </si>
+  <si>
+    <t>TS01</t>
+  </si>
+  <si>
+    <t>Lógica</t>
+  </si>
+  <si>
+    <t>Todos los meses</t>
+  </si>
+  <si>
+    <t>train$training</t>
+  </si>
+  <si>
+    <t>202105, 202104, 202103, 202102, 202101, 202012, 202011, 202010, 202009, 202008, 202007, 202006, 202005, 202004, 202003, 202002, 202001, 201912, 201911, 201910, 201909, 201908, 201907</t>
+  </si>
+  <si>
+    <t>train$validation</t>
+  </si>
+  <si>
+    <t>train$testing</t>
+  </si>
+  <si>
+    <t>undersampling</t>
+  </si>
+  <si>
+    <t>TS02</t>
+  </si>
+  <si>
+    <t>sin pandemia</t>
+  </si>
+  <si>
+    <t>202107, 202106, 202105, 202104, 202103, 202102, 202101, 202012, 202011, 202010, 202009, 202008, 202002, 202001, 201912, 201911, 201910, 201909</t>
+  </si>
+  <si>
+    <t>202107, 202106, 202105, 202104, 202103, 202102, 202101, 202012, 202011, 202010, 202009, 202008, 202007, 202006, 202005, 202004, 202003, 202002, 202001, 201912, 201911, 201910, 201909</t>
+  </si>
+  <si>
+    <t>202105, 202104, 202103, 202102, 202101, 202012, 202011, 202010, 202009, 202008, 202002, 202001, 201912, 201911, 201910, 201909, 201908, 201907</t>
+  </si>
+  <si>
+    <t>TS03</t>
+  </si>
+  <si>
+    <t>últimos meses</t>
+  </si>
+  <si>
+    <t>202107, 202106, 202105, 202104, 202103, 202102, 202101, 202012, 202011</t>
+  </si>
+  <si>
+    <t>202105, 202104, 202103, 202102, 202101, 202012, 202011</t>
+  </si>
+  <si>
+    <t>Hyperparameter Tuning</t>
+  </si>
+  <si>
+    <t>HT01</t>
+  </si>
+  <si>
+    <t>min_gain_to_split</t>
+  </si>
+  <si>
+    <t>lambda_l1</t>
+  </si>
+  <si>
+    <t>lambda_l2</t>
+  </si>
+  <si>
+    <t>en la BO</t>
+  </si>
+  <si>
+    <t>L= lower</t>
+  </si>
+  <si>
+    <t>U = upper</t>
+  </si>
+  <si>
+    <t>L.learning_rate</t>
+  </si>
+  <si>
+    <t>U.learning_rate</t>
+  </si>
+  <si>
+    <t>L.feature_fraction</t>
+  </si>
+  <si>
+    <t>U.feature_fraction</t>
+  </si>
+  <si>
+    <t>L.num_leaves</t>
+  </si>
+  <si>
+    <t>U.num_leaves</t>
+  </si>
+  <si>
+    <t>L.min_data_in_leaf</t>
+  </si>
+  <si>
+    <t>U.min_data_in_leaf</t>
+  </si>
+  <si>
+    <t>L.min_gain_to_split</t>
+  </si>
+  <si>
+    <t>U.min_gain_to_split</t>
+  </si>
+  <si>
+    <t>L.lambda_l1</t>
+  </si>
+  <si>
+    <t>U.lambda_l1</t>
+  </si>
+  <si>
+    <t>L.lambda_l2</t>
+  </si>
+  <si>
+    <t>U.lamda_l2</t>
+  </si>
+  <si>
+    <t>fijo</t>
+  </si>
+  <si>
+    <t>HT02</t>
   </si>
 </sst>
 </file>
@@ -127,6 +307,72 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{8B1A6007-7516-4CF7-908D-9706FCDAFDFA}" name="Table1" displayName="Table1" ref="A1:L2" totalsRowShown="0">
+  <autoFilter ref="A1:L2" xr:uid="{8B1A6007-7516-4CF7-908D-9706FCDAFDFA}"/>
+  <tableColumns count="12">
+    <tableColumn id="1" xr3:uid="{79E439E9-1F3D-4DD1-A524-74B46EAC0444}" name="Versión"/>
+    <tableColumn id="2" xr3:uid="{3656E2E4-440F-4CB1-8D1D-BAD848F4B0BE}" name="num.trees"/>
+    <tableColumn id="3" xr3:uid="{10FB91EE-262C-4F4E-8AF1-3E07C56E273D}" name="max.depth"/>
+    <tableColumn id="4" xr3:uid="{77E57216-EDE3-47A6-AF17-E3FD024CD8C4}" name="min.node.size"/>
+    <tableColumn id="5" xr3:uid="{4BE25C28-31B2-43DA-AE14-E051C7467A2E}" name="mtry"/>
+    <tableColumn id="6" xr3:uid="{67D9D5C2-E201-4851-83D1-A2C9F6200B9F}" name="semilla"/>
+    <tableColumn id="7" xr3:uid="{8DC1040B-4CDA-467B-A151-7A711098FE28}" name="Canarios"/>
+    <tableColumn id="8" xr3:uid="{6B7AB7C8-A54F-433D-9147-343E34CAA77F}" name="lag1"/>
+    <tableColumn id="9" xr3:uid="{0D6D7043-02C8-49D9-9448-0B967821482C}" name="lag2"/>
+    <tableColumn id="10" xr3:uid="{39786EDE-2AE2-47D2-9FCF-B04B548A9E52}" name="lag3"/>
+    <tableColumn id="11" xr3:uid="{3D7C81A1-7871-4F5B-A042-4EE0E4805AED}" name="Tendencias1"/>
+    <tableColumn id="12" xr3:uid="{AD83C31A-FBA4-4767-957C-932A355E01B8}" name="Tendencias2"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{F89A03AB-8558-4D10-8449-88C06748FF2C}" name="Table2" displayName="Table2" ref="A2:I5" totalsRowShown="0">
+  <autoFilter ref="A2:I5" xr:uid="{F89A03AB-8558-4D10-8449-88C06748FF2C}"/>
+  <tableColumns count="9">
+    <tableColumn id="1" xr3:uid="{DAE6D94B-DCFF-47EE-966B-864121FE5761}" name="Versión"/>
+    <tableColumn id="2" xr3:uid="{C1B9D022-5C7D-4509-9BF0-E376BEF906F1}" name="Lógica"/>
+    <tableColumn id="3" xr3:uid="{EE8EBAD2-1BFE-4E53-90F4-FB5A06D4EFC1}" name="future"/>
+    <tableColumn id="4" xr3:uid="{87D2C18E-0409-417B-8BDA-330E128F91B9}" name="final_train"/>
+    <tableColumn id="5" xr3:uid="{B4FF2FC7-A2AC-4434-9501-216A504C9F10}" name="train$training"/>
+    <tableColumn id="6" xr3:uid="{9142C7A9-B7EB-4340-9671-62F2526D6F31}" name="train$validation"/>
+    <tableColumn id="7" xr3:uid="{833E32C7-F155-4C70-A730-2AA8B24D3171}" name="train$testing"/>
+    <tableColumn id="8" xr3:uid="{40D4ADD3-2752-40E1-B976-232C611B14EF}" name="undersampling"/>
+    <tableColumn id="9" xr3:uid="{AAC45FF3-95E6-4BE4-B435-BE77BD697570}" name="semilla"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{7703B3D9-0B34-4519-B696-ABB45499F4F2}" name="Table3" displayName="Table3" ref="A2:R4" totalsRowShown="0">
+  <autoFilter ref="A2:R4" xr:uid="{7703B3D9-0B34-4519-B696-ABB45499F4F2}"/>
+  <tableColumns count="18">
+    <tableColumn id="1" xr3:uid="{39B7B839-80E2-43F4-A1D2-24642327E71D}" name="Versión"/>
+    <tableColumn id="2" xr3:uid="{670B7823-0753-4655-8D3F-73D0A2AFBE2E}" name="min_gain_to_split"/>
+    <tableColumn id="3" xr3:uid="{48A8E485-CDF6-43F8-9238-D6D74F95D3D5}" name="lambda_l1"/>
+    <tableColumn id="4" xr3:uid="{DCA7A87E-39FE-433C-85E5-51356B8268AB}" name="lambda_l2"/>
+    <tableColumn id="5" xr3:uid="{A628446C-11F8-499D-B592-27FC466EBA3E}" name="L.learning_rate"/>
+    <tableColumn id="6" xr3:uid="{0D3A1DD9-071E-41B6-B8A5-D3907E5E7CD9}" name="U.learning_rate"/>
+    <tableColumn id="7" xr3:uid="{03D06CCA-554B-4B53-9DB3-C5C874A310BA}" name="L.feature_fraction"/>
+    <tableColumn id="8" xr3:uid="{6F93BC78-CF9A-4EDC-9313-293CB2C47E48}" name="U.feature_fraction"/>
+    <tableColumn id="9" xr3:uid="{345D71FC-B7C0-4E5A-A356-0F819D0C208D}" name="L.num_leaves"/>
+    <tableColumn id="10" xr3:uid="{FB145E48-18CE-47BF-A0C5-3BCAC6CF618F}" name="U.num_leaves"/>
+    <tableColumn id="11" xr3:uid="{67767A91-8872-489D-B4B4-80AF2819CD42}" name="L.min_data_in_leaf"/>
+    <tableColumn id="12" xr3:uid="{82C8833F-AB3E-4171-A771-3E5A01103ABC}" name="U.min_data_in_leaf"/>
+    <tableColumn id="13" xr3:uid="{551556B9-9E71-4082-AD99-2C7827FF272D}" name="L.min_gain_to_split"/>
+    <tableColumn id="14" xr3:uid="{DB2D496E-4886-4F59-85DA-2510BF5DD2FB}" name="U.min_gain_to_split"/>
+    <tableColumn id="15" xr3:uid="{FF6D9AAC-B21D-47E5-95CF-57692E30CDE2}" name="L.lambda_l1"/>
+    <tableColumn id="16" xr3:uid="{300F9E77-144E-48ED-BA13-CDD1EC17C687}" name="U.lambda_l1"/>
+    <tableColumn id="17" xr3:uid="{E05BCE8F-4839-443F-A663-C290989F7E6C}" name="L.lambda_l2"/>
+    <tableColumn id="18" xr3:uid="{FAC398B2-1EB2-4654-934E-7564E3D32235}" name="U.lamda_l2"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -392,10 +638,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J4"/>
+  <dimension ref="A1:J8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A9" sqref="A9:L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -447,7 +693,479 @@
         <v>12</v>
       </c>
     </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>14</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F6DC643-BAFD-4FBD-9022-C3B409821E33}">
+  <dimension ref="A1:L2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K17" sqref="K17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="9.453125" customWidth="1"/>
+    <col min="2" max="2" width="11.6328125" customWidth="1"/>
+    <col min="3" max="3" width="12" customWidth="1"/>
+    <col min="4" max="4" width="14.90625" customWidth="1"/>
+    <col min="6" max="6" width="9" customWidth="1"/>
+    <col min="7" max="7" width="10.08984375" customWidth="1"/>
+    <col min="11" max="12" width="13.36328125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J1" t="s">
+        <v>24</v>
+      </c>
+      <c r="K1" t="s">
+        <v>25</v>
+      </c>
+      <c r="L1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2">
+        <v>250</v>
+      </c>
+      <c r="C2">
+        <v>10</v>
+      </c>
+      <c r="D2">
+        <v>600</v>
+      </c>
+      <c r="E2">
+        <v>50</v>
+      </c>
+      <c r="F2">
+        <v>10881</v>
+      </c>
+      <c r="G2">
+        <v>0.999</v>
+      </c>
+      <c r="H2" t="b">
+        <v>1</v>
+      </c>
+      <c r="I2" t="b">
+        <v>1</v>
+      </c>
+      <c r="J2" t="b">
+        <v>1</v>
+      </c>
+      <c r="K2" t="s">
+        <v>27</v>
+      </c>
+      <c r="L2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB023B04-9609-4E26-B20D-8F91BA592A57}">
+  <dimension ref="A1:I5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F30" sqref="F30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="9.453125" customWidth="1"/>
+    <col min="4" max="4" width="11.6328125" customWidth="1"/>
+    <col min="5" max="5" width="14.36328125" customWidth="1"/>
+    <col min="6" max="6" width="16.26953125" customWidth="1"/>
+    <col min="7" max="7" width="13.6328125" customWidth="1"/>
+    <col min="8" max="8" width="15.54296875" customWidth="1"/>
+    <col min="9" max="9" width="9" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E2" t="s">
+        <v>34</v>
+      </c>
+      <c r="F2" t="s">
+        <v>36</v>
+      </c>
+      <c r="G2" t="s">
+        <v>37</v>
+      </c>
+      <c r="H2" t="s">
+        <v>38</v>
+      </c>
+      <c r="I2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C3">
+        <v>202109</v>
+      </c>
+      <c r="D3" t="s">
+        <v>42</v>
+      </c>
+      <c r="E3" t="s">
+        <v>43</v>
+      </c>
+      <c r="F3">
+        <v>202106</v>
+      </c>
+      <c r="G3">
+        <v>202107</v>
+      </c>
+      <c r="H3">
+        <v>0.5</v>
+      </c>
+      <c r="I3">
+        <v>10881</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C4">
+        <v>202109</v>
+      </c>
+      <c r="D4" t="s">
+        <v>41</v>
+      </c>
+      <c r="E4" t="s">
+        <v>35</v>
+      </c>
+      <c r="F4">
+        <v>202106</v>
+      </c>
+      <c r="G4">
+        <v>202107</v>
+      </c>
+      <c r="H4">
+        <v>0.5</v>
+      </c>
+      <c r="I4">
+        <v>10881</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C5">
+        <v>202109</v>
+      </c>
+      <c r="D5" t="s">
+        <v>46</v>
+      </c>
+      <c r="E5" t="s">
+        <v>47</v>
+      </c>
+      <c r="F5">
+        <v>202106</v>
+      </c>
+      <c r="G5">
+        <v>202107</v>
+      </c>
+      <c r="H5">
+        <v>0.5</v>
+      </c>
+      <c r="I5">
+        <v>10881</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6179FBED-F10E-48FA-BB1B-5FF81E06BCFA}">
+  <dimension ref="A1:R4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="9.453125" customWidth="1"/>
+    <col min="2" max="2" width="18" customWidth="1"/>
+    <col min="3" max="4" width="11.6328125" customWidth="1"/>
+    <col min="5" max="5" width="15.54296875" customWidth="1"/>
+    <col min="6" max="6" width="16.08984375" customWidth="1"/>
+    <col min="7" max="7" width="18" customWidth="1"/>
+    <col min="8" max="8" width="18.54296875" customWidth="1"/>
+    <col min="9" max="9" width="14.453125" customWidth="1"/>
+    <col min="10" max="10" width="15" customWidth="1"/>
+    <col min="11" max="11" width="19" customWidth="1"/>
+    <col min="12" max="12" width="19.54296875" customWidth="1"/>
+    <col min="13" max="13" width="19.36328125" customWidth="1"/>
+    <col min="14" max="14" width="19.90625" customWidth="1"/>
+    <col min="15" max="15" width="13" customWidth="1"/>
+    <col min="16" max="16" width="13.54296875" customWidth="1"/>
+    <col min="17" max="17" width="13" customWidth="1"/>
+    <col min="18" max="18" width="12.453125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>48</v>
+      </c>
+      <c r="E1" t="s">
+        <v>54</v>
+      </c>
+      <c r="F1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C2" t="s">
+        <v>51</v>
+      </c>
+      <c r="D2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E2" t="s">
+        <v>56</v>
+      </c>
+      <c r="F2" t="s">
+        <v>57</v>
+      </c>
+      <c r="G2" t="s">
+        <v>58</v>
+      </c>
+      <c r="H2" t="s">
+        <v>59</v>
+      </c>
+      <c r="I2" t="s">
+        <v>60</v>
+      </c>
+      <c r="J2" t="s">
+        <v>61</v>
+      </c>
+      <c r="K2" t="s">
+        <v>62</v>
+      </c>
+      <c r="L2" t="s">
+        <v>63</v>
+      </c>
+      <c r="M2" t="s">
+        <v>64</v>
+      </c>
+      <c r="N2" t="s">
+        <v>65</v>
+      </c>
+      <c r="O2" t="s">
+        <v>66</v>
+      </c>
+      <c r="P2" t="s">
+        <v>67</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>68</v>
+      </c>
+      <c r="R2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B3" t="s">
+        <v>53</v>
+      </c>
+      <c r="C3" t="s">
+        <v>53</v>
+      </c>
+      <c r="D3" t="s">
+        <v>53</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>0.3</v>
+      </c>
+      <c r="G3">
+        <v>0.01</v>
+      </c>
+      <c r="H3">
+        <v>1</v>
+      </c>
+      <c r="I3">
+        <v>8</v>
+      </c>
+      <c r="J3">
+        <v>1024</v>
+      </c>
+      <c r="K3">
+        <v>80</v>
+      </c>
+      <c r="L3">
+        <v>50000</v>
+      </c>
+      <c r="M3">
+        <v>0</v>
+      </c>
+      <c r="N3">
+        <v>100</v>
+      </c>
+      <c r="O3">
+        <v>1E-4</v>
+      </c>
+      <c r="P3">
+        <v>100</v>
+      </c>
+      <c r="Q3">
+        <v>1E-4</v>
+      </c>
+      <c r="R3">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>71</v>
+      </c>
+      <c r="B4" t="s">
+        <v>53</v>
+      </c>
+      <c r="C4" t="s">
+        <v>53</v>
+      </c>
+      <c r="D4" t="s">
+        <v>70</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>0.3</v>
+      </c>
+      <c r="G4">
+        <v>0.01</v>
+      </c>
+      <c r="H4">
+        <v>1</v>
+      </c>
+      <c r="I4">
+        <v>8</v>
+      </c>
+      <c r="J4">
+        <v>1024</v>
+      </c>
+      <c r="K4">
+        <v>80</v>
+      </c>
+      <c r="L4">
+        <v>50000</v>
+      </c>
+      <c r="M4">
+        <v>0</v>
+      </c>
+      <c r="N4">
+        <v>0</v>
+      </c>
+      <c r="O4">
+        <v>1E-4</v>
+      </c>
+      <c r="P4">
+        <v>100</v>
+      </c>
+      <c r="Q4">
+        <v>1E-4</v>
+      </c>
+      <c r="R4">
+        <v>100</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
gamble first run third try
</commit_message>
<xml_diff>
--- a/src/workflow-colab/Editados/Apuestas/Config Workflow.xlsx
+++ b/src/workflow-colab/Editados/Apuestas/Config Workflow.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\guido\Desktop\CD03\dm2023a\src\workflow-colab\Editados\Apuestas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98B53FE8-65E4-4228-AFEE-C4D9D786F496}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F9CC40E-1817-4395-988B-7C936C031174}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15620" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="75">
   <si>
     <t>Archivo</t>
   </si>
@@ -255,6 +255,15 @@
   </si>
   <si>
     <t>HT02</t>
+  </si>
+  <si>
+    <t>FE02</t>
+  </si>
+  <si>
+    <t>Observación</t>
+  </si>
+  <si>
+    <t>Se cortó antes de tiempo</t>
   </si>
 </sst>
 </file>
@@ -310,9 +319,9 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{8B1A6007-7516-4CF7-908D-9706FCDAFDFA}" name="Table1" displayName="Table1" ref="A1:L2" totalsRowShown="0">
-  <autoFilter ref="A1:L2" xr:uid="{8B1A6007-7516-4CF7-908D-9706FCDAFDFA}"/>
-  <tableColumns count="12">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{8B1A6007-7516-4CF7-908D-9706FCDAFDFA}" name="Table1" displayName="Table1" ref="A1:M3" totalsRowShown="0">
+  <autoFilter ref="A1:M3" xr:uid="{8B1A6007-7516-4CF7-908D-9706FCDAFDFA}"/>
+  <tableColumns count="13">
     <tableColumn id="1" xr3:uid="{79E439E9-1F3D-4DD1-A524-74B46EAC0444}" name="Versión"/>
     <tableColumn id="2" xr3:uid="{3656E2E4-440F-4CB1-8D1D-BAD848F4B0BE}" name="num.trees"/>
     <tableColumn id="3" xr3:uid="{10FB91EE-262C-4F4E-8AF1-3E07C56E273D}" name="max.depth"/>
@@ -325,6 +334,7 @@
     <tableColumn id="10" xr3:uid="{39786EDE-2AE2-47D2-9FCF-B04B548A9E52}" name="lag3"/>
     <tableColumn id="11" xr3:uid="{3D7C81A1-7871-4F5B-A042-4EE0E4805AED}" name="Tendencias1"/>
     <tableColumn id="12" xr3:uid="{AD83C31A-FBA4-4767-957C-932A355E01B8}" name="Tendencias2"/>
+    <tableColumn id="13" xr3:uid="{BC773EFB-6D31-4921-BEDE-9DC8DC5DB42C}" name="Observación"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -705,10 +715,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F6DC643-BAFD-4FBD-9022-C3B409821E33}">
-  <dimension ref="A1:L2"/>
+  <dimension ref="A1:M3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K17" sqref="K17"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -722,7 +732,7 @@
     <col min="11" max="12" width="13.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>15</v>
       </c>
@@ -759,8 +769,11 @@
       <c r="L1" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>13</v>
       </c>
@@ -795,6 +808,47 @@
         <v>27</v>
       </c>
       <c r="L2" t="s">
+        <v>27</v>
+      </c>
+      <c r="M2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>72</v>
+      </c>
+      <c r="B3">
+        <v>200</v>
+      </c>
+      <c r="C3">
+        <v>9</v>
+      </c>
+      <c r="D3">
+        <v>600</v>
+      </c>
+      <c r="E3">
+        <v>50</v>
+      </c>
+      <c r="F3">
+        <v>10881</v>
+      </c>
+      <c r="G3">
+        <v>0.999</v>
+      </c>
+      <c r="H3" t="b">
+        <v>1</v>
+      </c>
+      <c r="I3" t="b">
+        <v>1</v>
+      </c>
+      <c r="J3" t="b">
+        <v>1</v>
+      </c>
+      <c r="K3" t="s">
+        <v>27</v>
+      </c>
+      <c r="L3" t="s">
         <v>27</v>
       </c>
     </row>
@@ -811,7 +865,7 @@
   <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F30" sqref="F30"/>
+      <selection activeCell="N13" sqref="N13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
gamble first run fourth try
</commit_message>
<xml_diff>
--- a/src/workflow-colab/Editados/Apuestas/Config Workflow.xlsx
+++ b/src/workflow-colab/Editados/Apuestas/Config Workflow.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\guido\Desktop\CD03\dm2023a\src\workflow-colab\Editados\Apuestas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F9CC40E-1817-4395-988B-7C936C031174}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60453AE3-9206-4BD5-9B1E-6BA91188636B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15620" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38280" yWindow="3165" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="81">
   <si>
     <t>Archivo</t>
   </si>
@@ -264,6 +264,24 @@
   </si>
   <si>
     <t>Se cortó antes de tiempo</t>
+  </si>
+  <si>
+    <t>TS04</t>
+  </si>
+  <si>
+    <t>future 202107, con pandemia</t>
+  </si>
+  <si>
+    <t>202103, 202102, 202101, 202012, 202011, 202010, 202009, 202008, 202007, 202006, 202005, 202004, 202003, 202002, 202001, 201912, 201911, 201910, 201909, 201908, 201907, 201906, 201905</t>
+  </si>
+  <si>
+    <t>FE01.02</t>
+  </si>
+  <si>
+    <t>FE03</t>
+  </si>
+  <si>
+    <t>FE04</t>
   </si>
 </sst>
 </file>
@@ -319,8 +337,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{8B1A6007-7516-4CF7-908D-9706FCDAFDFA}" name="Table1" displayName="Table1" ref="A1:M3" totalsRowShown="0">
-  <autoFilter ref="A1:M3" xr:uid="{8B1A6007-7516-4CF7-908D-9706FCDAFDFA}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{8B1A6007-7516-4CF7-908D-9706FCDAFDFA}" name="Table1" displayName="Table1" ref="A1:M6" totalsRowShown="0">
+  <autoFilter ref="A1:M6" xr:uid="{8B1A6007-7516-4CF7-908D-9706FCDAFDFA}"/>
   <tableColumns count="13">
     <tableColumn id="1" xr3:uid="{79E439E9-1F3D-4DD1-A524-74B46EAC0444}" name="Versión"/>
     <tableColumn id="2" xr3:uid="{3656E2E4-440F-4CB1-8D1D-BAD848F4B0BE}" name="num.trees"/>
@@ -341,8 +359,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{F89A03AB-8558-4D10-8449-88C06748FF2C}" name="Table2" displayName="Table2" ref="A2:I5" totalsRowShown="0">
-  <autoFilter ref="A2:I5" xr:uid="{F89A03AB-8558-4D10-8449-88C06748FF2C}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{F89A03AB-8558-4D10-8449-88C06748FF2C}" name="Table2" displayName="Table2" ref="A2:I6" totalsRowShown="0">
+  <autoFilter ref="A2:I6" xr:uid="{F89A03AB-8558-4D10-8449-88C06748FF2C}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{DAE6D94B-DCFF-47EE-966B-864121FE5761}" name="Versión"/>
     <tableColumn id="2" xr3:uid="{C1B9D022-5C7D-4509-9BF0-E376BEF906F1}" name="Lógica"/>
@@ -715,10 +733,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F6DC643-BAFD-4FBD-9022-C3B409821E33}">
-  <dimension ref="A1:M3"/>
+  <dimension ref="A1:M6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -816,7 +834,7 @@
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
       <c r="B3">
         <v>200</v>
@@ -849,6 +867,120 @@
         <v>27</v>
       </c>
       <c r="L3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>72</v>
+      </c>
+      <c r="B4">
+        <v>200</v>
+      </c>
+      <c r="C4">
+        <v>7</v>
+      </c>
+      <c r="D4">
+        <v>600</v>
+      </c>
+      <c r="E4">
+        <v>50</v>
+      </c>
+      <c r="F4">
+        <v>10881</v>
+      </c>
+      <c r="G4">
+        <v>0.999</v>
+      </c>
+      <c r="H4" t="b">
+        <v>1</v>
+      </c>
+      <c r="I4" t="b">
+        <v>1</v>
+      </c>
+      <c r="J4" t="b">
+        <v>1</v>
+      </c>
+      <c r="K4" t="s">
+        <v>27</v>
+      </c>
+      <c r="L4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>79</v>
+      </c>
+      <c r="B5">
+        <v>200</v>
+      </c>
+      <c r="C5">
+        <v>6</v>
+      </c>
+      <c r="D5">
+        <v>600</v>
+      </c>
+      <c r="E5">
+        <v>50</v>
+      </c>
+      <c r="F5">
+        <v>10881</v>
+      </c>
+      <c r="G5">
+        <v>0.999</v>
+      </c>
+      <c r="H5" t="b">
+        <v>1</v>
+      </c>
+      <c r="I5" t="b">
+        <v>1</v>
+      </c>
+      <c r="J5" t="b">
+        <v>1</v>
+      </c>
+      <c r="K5" t="s">
+        <v>27</v>
+      </c>
+      <c r="L5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>80</v>
+      </c>
+      <c r="B6">
+        <v>300</v>
+      </c>
+      <c r="C6">
+        <v>5</v>
+      </c>
+      <c r="D6">
+        <v>600</v>
+      </c>
+      <c r="E6">
+        <v>50</v>
+      </c>
+      <c r="F6">
+        <v>10881</v>
+      </c>
+      <c r="G6">
+        <v>0.999</v>
+      </c>
+      <c r="H6" t="b">
+        <v>1</v>
+      </c>
+      <c r="I6" t="b">
+        <v>1</v>
+      </c>
+      <c r="J6" t="b">
+        <v>1</v>
+      </c>
+      <c r="K6" t="s">
+        <v>27</v>
+      </c>
+      <c r="L6" t="s">
         <v>27</v>
       </c>
     </row>
@@ -862,10 +994,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB023B04-9609-4E26-B20D-8F91BA592A57}">
-  <dimension ref="A1:I5"/>
+  <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N13" sqref="N13"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -997,6 +1129,35 @@
         <v>0.5</v>
       </c>
       <c r="I5">
+        <v>10881</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>75</v>
+      </c>
+      <c r="B6" t="s">
+        <v>76</v>
+      </c>
+      <c r="C6">
+        <v>202107</v>
+      </c>
+      <c r="D6" t="s">
+        <v>35</v>
+      </c>
+      <c r="E6" t="s">
+        <v>77</v>
+      </c>
+      <c r="F6">
+        <v>202104</v>
+      </c>
+      <c r="G6">
+        <v>202105</v>
+      </c>
+      <c r="H6">
+        <v>0.5</v>
+      </c>
+      <c r="I6">
         <v>10881</v>
       </c>
     </row>

</xml_diff>

<commit_message>
gamble first run sixth try
</commit_message>
<xml_diff>
--- a/src/workflow-colab/Editados/Apuestas/Config Workflow.xlsx
+++ b/src/workflow-colab/Editados/Apuestas/Config Workflow.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\guido\Desktop\CD03\dm2023a\src\workflow-colab\Editados\Apuestas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60453AE3-9206-4BD5-9B1E-6BA91188636B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5E62F6D-AD82-44DB-B75E-1E2D545731F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="3165" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15620" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="87">
   <si>
     <t>Archivo</t>
   </si>
@@ -282,6 +282,24 @@
   </si>
   <si>
     <t>FE04</t>
+  </si>
+  <si>
+    <t>Todo TRUE - max y min</t>
+  </si>
+  <si>
+    <t>624gb ram insuficientes</t>
+  </si>
+  <si>
+    <t>FE05</t>
+  </si>
+  <si>
+    <t>FE06</t>
+  </si>
+  <si>
+    <t>FE07</t>
+  </si>
+  <si>
+    <t>FE08</t>
   </si>
 </sst>
 </file>
@@ -337,8 +355,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{8B1A6007-7516-4CF7-908D-9706FCDAFDFA}" name="Table1" displayName="Table1" ref="A1:M6" totalsRowShown="0">
-  <autoFilter ref="A1:M6" xr:uid="{8B1A6007-7516-4CF7-908D-9706FCDAFDFA}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{8B1A6007-7516-4CF7-908D-9706FCDAFDFA}" name="Table1" displayName="Table1" ref="A1:M10" totalsRowShown="0">
+  <autoFilter ref="A1:M10" xr:uid="{8B1A6007-7516-4CF7-908D-9706FCDAFDFA}"/>
   <tableColumns count="13">
     <tableColumn id="1" xr3:uid="{79E439E9-1F3D-4DD1-A524-74B46EAC0444}" name="Versión"/>
     <tableColumn id="2" xr3:uid="{3656E2E4-440F-4CB1-8D1D-BAD848F4B0BE}" name="num.trees"/>
@@ -733,10 +751,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F6DC643-BAFD-4FBD-9022-C3B409821E33}">
-  <dimension ref="A1:M6"/>
+  <dimension ref="A1:M10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="L20" sqref="L20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -869,6 +887,9 @@
       <c r="L3" t="s">
         <v>27</v>
       </c>
+      <c r="M3" t="s">
+        <v>82</v>
+      </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
@@ -907,6 +928,9 @@
       <c r="L4" t="s">
         <v>27</v>
       </c>
+      <c r="M4" t="s">
+        <v>82</v>
+      </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
@@ -945,6 +969,9 @@
       <c r="L5" t="s">
         <v>27</v>
       </c>
+      <c r="M5" t="s">
+        <v>82</v>
+      </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
@@ -982,6 +1009,161 @@
       </c>
       <c r="L6" t="s">
         <v>27</v>
+      </c>
+      <c r="M6" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>83</v>
+      </c>
+      <c r="B7">
+        <v>100</v>
+      </c>
+      <c r="C7">
+        <v>5</v>
+      </c>
+      <c r="D7">
+        <v>600</v>
+      </c>
+      <c r="E7">
+        <v>50</v>
+      </c>
+      <c r="F7">
+        <v>10881</v>
+      </c>
+      <c r="G7">
+        <v>0.999</v>
+      </c>
+      <c r="H7" t="b">
+        <v>1</v>
+      </c>
+      <c r="I7" t="b">
+        <v>1</v>
+      </c>
+      <c r="J7" t="b">
+        <v>1</v>
+      </c>
+      <c r="K7" t="s">
+        <v>81</v>
+      </c>
+      <c r="L7" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>84</v>
+      </c>
+      <c r="B8">
+        <v>100</v>
+      </c>
+      <c r="C8">
+        <v>4</v>
+      </c>
+      <c r="D8">
+        <v>600</v>
+      </c>
+      <c r="E8">
+        <v>50</v>
+      </c>
+      <c r="F8">
+        <v>10881</v>
+      </c>
+      <c r="G8">
+        <v>0.999</v>
+      </c>
+      <c r="H8" t="b">
+        <v>1</v>
+      </c>
+      <c r="I8" t="b">
+        <v>1</v>
+      </c>
+      <c r="J8" t="b">
+        <v>1</v>
+      </c>
+      <c r="K8" t="s">
+        <v>27</v>
+      </c>
+      <c r="L8" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>85</v>
+      </c>
+      <c r="B9">
+        <v>80</v>
+      </c>
+      <c r="C9">
+        <v>4</v>
+      </c>
+      <c r="D9">
+        <v>600</v>
+      </c>
+      <c r="E9">
+        <v>50</v>
+      </c>
+      <c r="F9">
+        <v>10881</v>
+      </c>
+      <c r="G9">
+        <v>0.999</v>
+      </c>
+      <c r="H9" t="b">
+        <v>1</v>
+      </c>
+      <c r="I9" t="b">
+        <v>1</v>
+      </c>
+      <c r="J9" t="b">
+        <v>1</v>
+      </c>
+      <c r="K9" t="s">
+        <v>81</v>
+      </c>
+      <c r="L9" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>86</v>
+      </c>
+      <c r="B10">
+        <v>80</v>
+      </c>
+      <c r="C10">
+        <v>8</v>
+      </c>
+      <c r="D10">
+        <v>500</v>
+      </c>
+      <c r="E10">
+        <v>40</v>
+      </c>
+      <c r="F10">
+        <v>10881</v>
+      </c>
+      <c r="G10">
+        <v>0.8</v>
+      </c>
+      <c r="H10" t="b">
+        <v>1</v>
+      </c>
+      <c r="I10" t="b">
+        <v>1</v>
+      </c>
+      <c r="J10" t="b">
+        <v>1</v>
+      </c>
+      <c r="K10" t="s">
+        <v>81</v>
+      </c>
+      <c r="L10" t="b">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
gamble first run, ZZs
</commit_message>
<xml_diff>
--- a/src/workflow-colab/Editados/Apuestas/Config Workflow.xlsx
+++ b/src/workflow-colab/Editados/Apuestas/Config Workflow.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\guido\Desktop\CD03\dm2023a\src\workflow-colab\Editados\Apuestas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5E62F6D-AD82-44DB-B75E-1E2D545731F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D63B246-54DC-4769-8254-FB7EF5BB7B72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15620" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="FE" sheetId="2" r:id="rId2"/>
     <sheet name="TS" sheetId="3" r:id="rId3"/>
     <sheet name="HT" sheetId="4" r:id="rId4"/>
+    <sheet name="ZZ" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="97">
   <si>
     <t>Archivo</t>
   </si>
@@ -83,9 +84,6 @@
     <t>FE01</t>
   </si>
   <si>
-    <t>Feature Engineering</t>
-  </si>
-  <si>
     <t>Versión</t>
   </si>
   <si>
@@ -300,6 +298,39 @@
   </si>
   <si>
     <t>FE08</t>
+  </si>
+  <si>
+    <t>FE</t>
+  </si>
+  <si>
+    <t>Final</t>
+  </si>
+  <si>
+    <t>ZZ01</t>
+  </si>
+  <si>
+    <t>Desde</t>
+  </si>
+  <si>
+    <t>Hasta</t>
+  </si>
+  <si>
+    <t>Salto</t>
+  </si>
+  <si>
+    <t>Rank</t>
+  </si>
+  <si>
+    <t>Semillas</t>
+  </si>
+  <si>
+    <t>108881, 262637, 541447, 678547, 848629</t>
+  </si>
+  <si>
+    <t>*podría agregar más rank</t>
+  </si>
+  <si>
+    <t>ZZ</t>
   </si>
 </sst>
 </file>
@@ -355,6 +386,19 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{F7D7D7A1-E25A-4312-B092-3FC812CAE881}" name="Table4" displayName="Table4" ref="A8:D13" totalsRowShown="0">
+  <autoFilter ref="A8:D13" xr:uid="{F7D7D7A1-E25A-4312-B092-3FC812CAE881}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{EE346C9F-4A34-4B95-BB20-852B9BAFD055}" name="FE"/>
+    <tableColumn id="2" xr3:uid="{8272D39F-3A5D-48DB-A1CE-ECEBD9F35F38}" name="TS"/>
+    <tableColumn id="3" xr3:uid="{C7398975-296E-49B9-88C0-FAAE9FED4EAC}" name="HT"/>
+    <tableColumn id="4" xr3:uid="{DFCBC839-40B5-40C9-A607-4E3ECDDCB7EC}" name="ZZ"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{8B1A6007-7516-4CF7-908D-9706FCDAFDFA}" name="Table1" displayName="Table1" ref="A1:M10" totalsRowShown="0">
   <autoFilter ref="A1:M10" xr:uid="{8B1A6007-7516-4CF7-908D-9706FCDAFDFA}"/>
   <tableColumns count="13">
@@ -376,7 +420,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{F89A03AB-8558-4D10-8449-88C06748FF2C}" name="Table2" displayName="Table2" ref="A2:I6" totalsRowShown="0">
   <autoFilter ref="A2:I6" xr:uid="{F89A03AB-8558-4D10-8449-88C06748FF2C}"/>
   <tableColumns count="9">
@@ -394,7 +438,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{7703B3D9-0B34-4519-B696-ABB45499F4F2}" name="Table3" displayName="Table3" ref="A2:R4" totalsRowShown="0">
   <autoFilter ref="A2:R4" xr:uid="{7703B3D9-0B34-4519-B696-ABB45499F4F2}"/>
   <tableColumns count="18">
@@ -416,6 +460,21 @@
     <tableColumn id="16" xr3:uid="{300F9E77-144E-48ED-BA13-CDD1EC17C687}" name="U.lambda_l1"/>
     <tableColumn id="17" xr3:uid="{E05BCE8F-4839-443F-A663-C290989F7E6C}" name="L.lambda_l2"/>
     <tableColumn id="18" xr3:uid="{FAC398B2-1EB2-4654-934E-7564E3D32235}" name="U.lamda_l2"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{3F2D2FD8-4692-4FD8-A896-05F164C82D2D}" name="Table5" displayName="Table5" ref="A2:F3" totalsRowShown="0">
+  <autoFilter ref="A2:F3" xr:uid="{3F2D2FD8-4692-4FD8-A896-05F164C82D2D}"/>
+  <tableColumns count="6">
+    <tableColumn id="1" xr3:uid="{D7FE12C4-036A-4E5D-B0DF-F6FE9AE5F6CE}" name="Versión"/>
+    <tableColumn id="2" xr3:uid="{5B3DEF63-03B8-42A3-AF49-C86C8EC7F86E}" name="Rank"/>
+    <tableColumn id="3" xr3:uid="{C81087D4-7C5E-4660-A26B-1E9C18AE5208}" name="Desde"/>
+    <tableColumn id="4" xr3:uid="{ED3B51A3-363A-4A68-81A9-5FB700397E5B}" name="Hasta"/>
+    <tableColumn id="5" xr3:uid="{7AD3D3E2-C6AA-422F-90A1-E9CC4A7A69E8}" name="Salto"/>
+    <tableColumn id="6" xr3:uid="{F06B0C0E-98EA-4163-BCB0-C1BC02D18481}" name="Semillas"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -684,10 +743,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J8"/>
+  <dimension ref="A1:J13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9:L10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -741,11 +800,69 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>14</v>
+        <v>86</v>
+      </c>
+      <c r="B8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>82</v>
+      </c>
+      <c r="B9" t="s">
+        <v>30</v>
+      </c>
+      <c r="C9" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>82</v>
+      </c>
+      <c r="B10" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>82</v>
+      </c>
+      <c r="B11" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>82</v>
+      </c>
+      <c r="B12" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>85</v>
+      </c>
+      <c r="B13" t="s">
+        <v>30</v>
+      </c>
+      <c r="C13" t="s">
+        <v>48</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
 
@@ -753,8 +870,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F6DC643-BAFD-4FBD-9022-C3B409821E33}">
   <dimension ref="A1:M10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L20" sqref="L20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M16" sqref="M16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -770,43 +887,43 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" t="s">
         <v>15</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>16</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>17</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>18</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>19</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>20</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>21</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>22</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>23</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>24</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>25</v>
       </c>
-      <c r="L1" t="s">
-        <v>26</v>
-      </c>
       <c r="M1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.35">
@@ -841,18 +958,18 @@
         <v>1</v>
       </c>
       <c r="K2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="L2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="M2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B3">
         <v>200</v>
@@ -882,18 +999,18 @@
         <v>1</v>
       </c>
       <c r="K3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="L3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="M3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B4">
         <v>200</v>
@@ -923,18 +1040,18 @@
         <v>1</v>
       </c>
       <c r="K4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="L4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="M4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B5">
         <v>200</v>
@@ -964,18 +1081,18 @@
         <v>1</v>
       </c>
       <c r="K5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="L5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="M5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B6">
         <v>300</v>
@@ -1005,18 +1122,18 @@
         <v>1</v>
       </c>
       <c r="K6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="L6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="M6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B7">
         <v>100</v>
@@ -1046,15 +1163,15 @@
         <v>1</v>
       </c>
       <c r="K7" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="L7" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B8">
         <v>100</v>
@@ -1084,15 +1201,15 @@
         <v>1</v>
       </c>
       <c r="K8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="L8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B9">
         <v>80</v>
@@ -1122,15 +1239,15 @@
         <v>1</v>
       </c>
       <c r="K9" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="L9" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B10">
         <v>80</v>
@@ -1160,7 +1277,7 @@
         <v>1</v>
       </c>
       <c r="K10" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="L10" t="b">
         <v>0</v>
@@ -1179,12 +1296,13 @@
   <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="9.453125" customWidth="1"/>
+    <col min="2" max="2" width="25.54296875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.6328125" customWidth="1"/>
     <col min="5" max="5" width="14.36328125" customWidth="1"/>
     <col min="6" max="6" width="16.26953125" customWidth="1"/>
@@ -1195,53 +1313,53 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D2" t="s">
         <v>29</v>
       </c>
-      <c r="D2" t="s">
-        <v>30</v>
-      </c>
       <c r="E2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F2" t="s">
+        <v>35</v>
+      </c>
+      <c r="G2" t="s">
         <v>36</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>37</v>
       </c>
-      <c r="H2" t="s">
-        <v>38</v>
-      </c>
       <c r="I2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C3">
         <v>202109</v>
       </c>
       <c r="D3" t="s">
+        <v>41</v>
+      </c>
+      <c r="E3" t="s">
         <v>42</v>
-      </c>
-      <c r="E3" t="s">
-        <v>43</v>
       </c>
       <c r="F3">
         <v>202106</v>
@@ -1258,19 +1376,19 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B4" t="s">
         <v>39</v>
-      </c>
-      <c r="B4" t="s">
-        <v>40</v>
       </c>
       <c r="C4">
         <v>202109</v>
       </c>
       <c r="D4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F4">
         <v>202106</v>
@@ -1287,19 +1405,19 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
+        <v>43</v>
+      </c>
+      <c r="B5" t="s">
         <v>44</v>
-      </c>
-      <c r="B5" t="s">
-        <v>45</v>
       </c>
       <c r="C5">
         <v>202109</v>
       </c>
       <c r="D5" t="s">
+        <v>45</v>
+      </c>
+      <c r="E5" t="s">
         <v>46</v>
-      </c>
-      <c r="E5" t="s">
-        <v>47</v>
       </c>
       <c r="F5">
         <v>202106</v>
@@ -1316,19 +1434,19 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
+        <v>74</v>
+      </c>
+      <c r="B6" t="s">
         <v>75</v>
-      </c>
-      <c r="B6" t="s">
-        <v>76</v>
       </c>
       <c r="C6">
         <v>202107</v>
       </c>
       <c r="D6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F6">
         <v>202104</v>
@@ -1356,7 +1474,7 @@
   <dimension ref="A1:R4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1382,83 +1500,83 @@
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E1" t="s">
+        <v>53</v>
+      </c>
+      <c r="F1" t="s">
         <v>54</v>
-      </c>
-      <c r="F1" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C2" t="s">
         <v>50</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>51</v>
       </c>
-      <c r="D2" t="s">
-        <v>52</v>
-      </c>
       <c r="E2" t="s">
+        <v>55</v>
+      </c>
+      <c r="F2" t="s">
         <v>56</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>57</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>58</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>59</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>60</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>61</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>62</v>
       </c>
-      <c r="L2" t="s">
+      <c r="M2" t="s">
         <v>63</v>
       </c>
-      <c r="M2" t="s">
+      <c r="N2" t="s">
         <v>64</v>
       </c>
-      <c r="N2" t="s">
+      <c r="O2" t="s">
         <v>65</v>
       </c>
-      <c r="O2" t="s">
+      <c r="P2" t="s">
         <v>66</v>
       </c>
-      <c r="P2" t="s">
+      <c r="Q2" t="s">
         <v>67</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="R2" t="s">
         <v>68</v>
-      </c>
-      <c r="R2" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E3">
         <v>0</v>
@@ -1505,16 +1623,16 @@
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E4">
         <v>0</v>
@@ -1557,6 +1675,76 @@
       </c>
       <c r="R4">
         <v>100</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5F24F4F-8ECA-4E50-9A38-A6F7C662B08E}">
+  <dimension ref="A1:K3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M11" sqref="M11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="9.1796875" customWidth="1"/>
+    <col min="6" max="6" width="9.54296875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" t="s">
+        <v>92</v>
+      </c>
+      <c r="C2" t="s">
+        <v>89</v>
+      </c>
+      <c r="D2" t="s">
+        <v>90</v>
+      </c>
+      <c r="E2" t="s">
+        <v>91</v>
+      </c>
+      <c r="F2" t="s">
+        <v>93</v>
+      </c>
+      <c r="K2" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>88</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>10500</v>
+      </c>
+      <c r="D3">
+        <v>12000</v>
+      </c>
+      <c r="E3">
+        <v>100</v>
+      </c>
+      <c r="F3" t="s">
+        <v>94</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
gamble FE10 a FE12
</commit_message>
<xml_diff>
--- a/src/workflow-colab/Editados/Apuestas/Config Workflow.xlsx
+++ b/src/workflow-colab/Editados/Apuestas/Config Workflow.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\guido\Desktop\CD03\dm2023a\src\workflow-colab\Editados\Apuestas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D230A7B-349B-41ED-891A-0380D6D2227D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7F6B2D9-A442-409B-B3FE-159A0254DCB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15620" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="107">
   <si>
     <t>Archivo</t>
   </si>
@@ -334,6 +334,33 @@
   </si>
   <si>
     <t>Todo TRUE - min, max, promedio</t>
+  </si>
+  <si>
+    <t>FE09</t>
+  </si>
+  <si>
+    <t>TS05</t>
+  </si>
+  <si>
+    <t>OK</t>
+  </si>
+  <si>
+    <t>Parece que terminó, no 100% seguro</t>
+  </si>
+  <si>
+    <t>FE10</t>
+  </si>
+  <si>
+    <t>FE11</t>
+  </si>
+  <si>
+    <t>FE12</t>
+  </si>
+  <si>
+    <t>Estado</t>
+  </si>
+  <si>
+    <t>corriendo</t>
   </si>
 </sst>
 </file>
@@ -369,9 +396,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -390,21 +416,22 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{F7D7D7A1-E25A-4312-B092-3FC812CAE881}" name="Table4" displayName="Table4" ref="A8:D13" totalsRowShown="0">
-  <autoFilter ref="A8:D13" xr:uid="{F7D7D7A1-E25A-4312-B092-3FC812CAE881}"/>
-  <tableColumns count="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{F7D7D7A1-E25A-4312-B092-3FC812CAE881}" name="Table4" displayName="Table4" ref="A8:E18" totalsRowShown="0">
+  <autoFilter ref="A8:E18" xr:uid="{F7D7D7A1-E25A-4312-B092-3FC812CAE881}"/>
+  <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{EE346C9F-4A34-4B95-BB20-852B9BAFD055}" name="FE"/>
     <tableColumn id="2" xr3:uid="{8272D39F-3A5D-48DB-A1CE-ECEBD9F35F38}" name="TS"/>
     <tableColumn id="3" xr3:uid="{C7398975-296E-49B9-88C0-FAAE9FED4EAC}" name="HT"/>
     <tableColumn id="4" xr3:uid="{DFCBC839-40B5-40C9-A607-4E3ECDDCB7EC}" name="ZZ"/>
+    <tableColumn id="5" xr3:uid="{878234D6-BDFA-4FF0-A9B0-541F42FAB0F1}" name="Estado"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{8B1A6007-7516-4CF7-908D-9706FCDAFDFA}" name="Table1" displayName="Table1" ref="A1:M11" totalsRowShown="0">
-  <autoFilter ref="A1:M11" xr:uid="{8B1A6007-7516-4CF7-908D-9706FCDAFDFA}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{8B1A6007-7516-4CF7-908D-9706FCDAFDFA}" name="Table1" displayName="Table1" ref="A1:M14" totalsRowShown="0">
+  <autoFilter ref="A1:M14" xr:uid="{8B1A6007-7516-4CF7-908D-9706FCDAFDFA}"/>
   <tableColumns count="13">
     <tableColumn id="1" xr3:uid="{79E439E9-1F3D-4DD1-A524-74B46EAC0444}" name="Versión"/>
     <tableColumn id="2" xr3:uid="{3656E2E4-440F-4CB1-8D1D-BAD848F4B0BE}" name="num.trees"/>
@@ -747,10 +774,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J13"/>
+  <dimension ref="A1:J18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -815,6 +842,9 @@
       <c r="D8" t="s">
         <v>96</v>
       </c>
+      <c r="E8" t="s">
+        <v>105</v>
+      </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
@@ -826,7 +856,7 @@
       <c r="C9" t="s">
         <v>48</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="D9" t="s">
         <v>88</v>
       </c>
     </row>
@@ -851,7 +881,7 @@
       <c r="C11" t="s">
         <v>48</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="D11" t="s">
         <v>88</v>
       </c>
     </row>
@@ -878,6 +908,49 @@
       </c>
       <c r="D13" t="s">
         <v>88</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>98</v>
+      </c>
+      <c r="F14" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>82</v>
+      </c>
+      <c r="B15" t="s">
+        <v>99</v>
+      </c>
+      <c r="F15" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>102</v>
+      </c>
+      <c r="E16" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>103</v>
+      </c>
+      <c r="E17" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>104</v>
+      </c>
+      <c r="E18" t="s">
+        <v>106</v>
       </c>
     </row>
   </sheetData>
@@ -891,10 +964,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F6DC643-BAFD-4FBD-9022-C3B409821E33}">
-  <dimension ref="A1:M11"/>
+  <dimension ref="A1:M14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J26" sqref="J26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1308,7 +1381,7 @@
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>85</v>
+        <v>98</v>
       </c>
       <c r="B11">
         <v>200</v>
@@ -1342,6 +1415,120 @@
       </c>
       <c r="L11" t="s">
         <v>97</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>102</v>
+      </c>
+      <c r="B12">
+        <v>300</v>
+      </c>
+      <c r="C12">
+        <v>11</v>
+      </c>
+      <c r="D12">
+        <v>400</v>
+      </c>
+      <c r="E12">
+        <v>40</v>
+      </c>
+      <c r="F12">
+        <v>10881</v>
+      </c>
+      <c r="G12">
+        <v>0.25</v>
+      </c>
+      <c r="H12" t="b">
+        <v>1</v>
+      </c>
+      <c r="I12" t="b">
+        <v>1</v>
+      </c>
+      <c r="J12" t="b">
+        <v>1</v>
+      </c>
+      <c r="K12" t="s">
+        <v>26</v>
+      </c>
+      <c r="L12" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>103</v>
+      </c>
+      <c r="B13">
+        <v>300</v>
+      </c>
+      <c r="C13">
+        <v>11</v>
+      </c>
+      <c r="D13">
+        <v>600</v>
+      </c>
+      <c r="E13">
+        <v>40</v>
+      </c>
+      <c r="F13">
+        <v>10881</v>
+      </c>
+      <c r="G13">
+        <v>0.25</v>
+      </c>
+      <c r="H13" t="b">
+        <v>1</v>
+      </c>
+      <c r="I13" t="b">
+        <v>1</v>
+      </c>
+      <c r="J13" t="b">
+        <v>1</v>
+      </c>
+      <c r="K13" t="s">
+        <v>26</v>
+      </c>
+      <c r="L13" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>104</v>
+      </c>
+      <c r="B14">
+        <v>300</v>
+      </c>
+      <c r="C14">
+        <v>11</v>
+      </c>
+      <c r="D14">
+        <v>800</v>
+      </c>
+      <c r="E14">
+        <v>40</v>
+      </c>
+      <c r="F14">
+        <v>10881</v>
+      </c>
+      <c r="G14">
+        <v>0.25</v>
+      </c>
+      <c r="H14" t="b">
+        <v>1</v>
+      </c>
+      <c r="I14" t="b">
+        <v>1</v>
+      </c>
+      <c r="J14" t="b">
+        <v>1</v>
+      </c>
+      <c r="K14" t="s">
+        <v>26</v>
+      </c>
+      <c r="L14" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -1357,7 +1544,7 @@
   <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1524,7 +1711,7 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>30</v>
+        <v>99</v>
       </c>
       <c r="B7" t="s">
         <v>32</v>

</xml_diff>

<commit_message>
gamble fe10 to fe15 again
</commit_message>
<xml_diff>
--- a/src/workflow-colab/Editados/Apuestas/Config Workflow.xlsx
+++ b/src/workflow-colab/Editados/Apuestas/Config Workflow.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\guido\Desktop\CD03\dm2023a\src\workflow-colab\Editados\Apuestas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D47A4DD-176E-4327-87C1-3D1653B28C37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAA3461C-CE29-4FC1-BEF6-BF58D6394B1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15620" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15620" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -807,7 +807,7 @@
   <dimension ref="A1:J21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E16" sqref="E16:E18"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -964,7 +964,7 @@
         <v>102</v>
       </c>
       <c r="E16" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.35">
@@ -1020,8 +1020,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F6DC643-BAFD-4FBD-9022-C3B409821E33}">
   <dimension ref="A1:M17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12:B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1476,13 +1476,13 @@
         <v>102</v>
       </c>
       <c r="B12">
+        <v>200</v>
+      </c>
+      <c r="C12">
+        <v>10</v>
+      </c>
+      <c r="D12">
         <v>300</v>
-      </c>
-      <c r="C12">
-        <v>11</v>
-      </c>
-      <c r="D12">
-        <v>400</v>
       </c>
       <c r="E12">
         <v>40</v>
@@ -1514,13 +1514,13 @@
         <v>103</v>
       </c>
       <c r="B13">
-        <v>300</v>
+        <v>200</v>
       </c>
       <c r="C13">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D13">
-        <v>600</v>
+        <v>400</v>
       </c>
       <c r="E13">
         <v>40</v>
@@ -1552,13 +1552,13 @@
         <v>104</v>
       </c>
       <c r="B14">
-        <v>300</v>
+        <v>200</v>
       </c>
       <c r="C14">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D14">
-        <v>800</v>
+        <v>600</v>
       </c>
       <c r="E14">
         <v>40</v>
@@ -1590,13 +1590,13 @@
         <v>107</v>
       </c>
       <c r="B15">
-        <v>300</v>
+        <v>200</v>
       </c>
       <c r="C15">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D15">
-        <v>1000</v>
+        <v>800</v>
       </c>
       <c r="E15">
         <v>40</v>
@@ -1628,13 +1628,13 @@
         <v>108</v>
       </c>
       <c r="B16">
-        <v>300</v>
+        <v>200</v>
       </c>
       <c r="C16">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D16">
-        <v>1200</v>
+        <v>1000</v>
       </c>
       <c r="E16">
         <v>40</v>
@@ -1666,13 +1666,13 @@
         <v>109</v>
       </c>
       <c r="B17">
-        <v>300</v>
+        <v>200</v>
       </c>
       <c r="C17">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D17">
-        <v>300</v>
+        <v>1200</v>
       </c>
       <c r="E17">
         <v>40</v>
@@ -1711,7 +1711,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB023B04-9609-4E26-B20D-8F91BA592A57}">
   <dimension ref="A1:I8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="O18" sqref="O18"/>
     </sheetView>
   </sheetViews>

</xml_diff>